<commit_message>
eg dataset done Tutorial on totals PCA
</commit_message>
<xml_diff>
--- a/eg_data/VVKAJ/VVKAJ_Items_f_s_m_summ.xlsx
+++ b/eg_data/VVKAJ/VVKAJ_Items_f_s_m_summ.xlsx
@@ -1,34 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\dietary_patterns\eg_data\VVKAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E5EE9-5837-4DA1-BA6F-0699D5C49611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C4E726-49C5-406E-9C31-86CB7BAECAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25095" yWindow="-2625" windowWidth="16950" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="345" windowWidth="15900" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -789,13 +779,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -916,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>2.0329670329670302</v>
+        <v>2.02507374631268</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -925,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="H5">
-        <v>0.82966143313066998</v>
+        <v>0.835488470425364</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1095,10 +1087,10 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>2.5362637362637401</v>
+        <v>2.4601769911504401</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -1107,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="H12">
-        <v>1.23205323447517</v>
+        <v>1.19725484797149</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1150,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>2.9587020648967601</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1159,7 +1151,7 @@
         <v>7</v>
       </c>
       <c r="H14">
-        <v>1.6738465026810101</v>
+        <v>1.6145770869168501</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>2.6417582417582399</v>
+        <v>2.7772861356932199</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1237,7 +1229,7 @@
         <v>11</v>
       </c>
       <c r="H17">
-        <v>2.4443617552979799</v>
+        <v>2.4721103736269399</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1254,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>7.2659340659340703</v>
+        <v>7.1814159292035402</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -1263,7 +1255,7 @@
         <v>22</v>
       </c>
       <c r="H18">
-        <v>4.1927202429080204</v>
+        <v>4.2587447337333897</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1.1582417582417599</v>
+        <v>1.1607669616519201</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1289,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>0.36536926407877501</v>
+        <v>0.36758704830240801</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1332,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="E21">
-        <v>8.5362637362637397</v>
+        <v>8.53097345132743</v>
       </c>
       <c r="F21">
         <v>12</v>
@@ -1341,7 +1333,7 @@
         <v>24</v>
       </c>
       <c r="H21">
-        <v>5.10099576707848</v>
+        <v>5.1363749807781902</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,16 +1341,16 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>11111000</v>
+        <v>11100000</v>
       </c>
       <c r="C22">
-        <v>41601070</v>
+        <v>41420300</v>
       </c>
       <c r="D22">
-        <v>63223020</v>
+        <v>63105010</v>
       </c>
       <c r="E22">
-        <v>60984825.224175803</v>
+        <v>60118100.768436603</v>
       </c>
       <c r="F22">
         <v>75302080</v>
@@ -1367,7 +1359,7 @@
         <v>95230020</v>
       </c>
       <c r="H22">
-        <v>24150964.6893587</v>
+        <v>24454655.043572199</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1404,22 +1396,22 @@
         <v>2.0799999999999999E-2</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>3.0878775164835202</v>
+        <v>3.3939634808274302</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>42.524999999999999</v>
+        <v>56.7</v>
       </c>
       <c r="H24">
-        <v>4.7907559421561503</v>
+        <v>5.6580184361565102</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,16 +1428,16 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1475.29498525074</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1000250</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>38414.369824286499</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1462,16 +1454,16 @@
         <v>30000</v>
       </c>
       <c r="E26">
-        <v>31391.9406593407</v>
+        <v>32279.247787610599</v>
       </c>
       <c r="F26">
-        <v>61009</v>
+        <v>61031.5</v>
       </c>
       <c r="G26">
-        <v>64696</v>
+        <v>64715</v>
       </c>
       <c r="H26">
-        <v>22267.430581634799</v>
+        <v>22446.7278620736</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,22 +1474,22 @@
         <v>0.3</v>
       </c>
       <c r="C27">
-        <v>28.175000000000001</v>
+        <v>28.35</v>
       </c>
       <c r="D27">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27">
-        <v>132.68475036629999</v>
+        <v>131.564713903643</v>
       </c>
       <c r="F27">
-        <v>228.4</v>
+        <v>226.8</v>
       </c>
       <c r="G27">
-        <v>720</v>
+        <v>740</v>
       </c>
       <c r="H27">
-        <v>129.12695464019899</v>
+        <v>131.70352594404201</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1508,22 +1500,22 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>10.425000000000001</v>
+        <v>10.025</v>
       </c>
       <c r="D28">
         <v>76.8</v>
       </c>
       <c r="E28">
-        <v>130.43919619816899</v>
+        <v>130.154271870305</v>
       </c>
       <c r="F28">
-        <v>173.3</v>
+        <v>167.7808125</v>
       </c>
       <c r="G28">
         <v>1196.79</v>
       </c>
       <c r="H28">
-        <v>167.82007735187699</v>
+        <v>166.20636287843101</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1534,22 +1526,22 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0.33954000000000001</v>
+        <v>0.32338125000000001</v>
       </c>
       <c r="D29">
-        <v>1.81104</v>
+        <v>1.975325</v>
       </c>
       <c r="E29">
-        <v>6.1819434487325999</v>
+        <v>6.3208139007581101</v>
       </c>
       <c r="F29">
-        <v>6.500985</v>
+        <v>7.3145749999999996</v>
       </c>
       <c r="G29">
-        <v>85.322159999999997</v>
+        <v>92.058120000000002</v>
       </c>
       <c r="H29">
-        <v>10.604194829077301</v>
+        <v>10.971567077338699</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1560,22 +1552,22 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>8.7421874999999996E-2</v>
+        <v>7.2281250000000005E-2</v>
       </c>
       <c r="D30">
-        <v>1.6234999999999999</v>
+        <v>1.6253375000000001</v>
       </c>
       <c r="E30">
-        <v>6.0214222685750904</v>
+        <v>5.9999537129159304</v>
       </c>
       <c r="F30">
-        <v>7.4608999999999996</v>
+        <v>7.5209999999999999</v>
       </c>
       <c r="G30">
         <v>70.439599999999999</v>
       </c>
       <c r="H30">
-        <v>9.7842937164828303</v>
+        <v>9.8520170615273894</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1586,22 +1578,22 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0.78885937500000003</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="D31">
-        <v>4.11355</v>
+        <v>3.9997425</v>
       </c>
       <c r="E31">
-        <v>13.001275961923101</v>
+        <v>12.829355063126799</v>
       </c>
       <c r="F31">
-        <v>17.303999999999998</v>
+        <v>17.2990125</v>
       </c>
       <c r="G31">
         <v>132.77279999999999</v>
       </c>
       <c r="H31">
-        <v>20.201452474115101</v>
+        <v>19.799115566545598</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1612,22 +1604,22 @@
         <v>4.6000000000000001E-4</v>
       </c>
       <c r="C32">
-        <v>15.9702454166666</v>
+        <v>15.446999999999999</v>
       </c>
       <c r="D32">
-        <v>53.865000000000002</v>
+        <v>52.356000000000002</v>
       </c>
       <c r="E32">
-        <v>105.850050752201</v>
+        <v>104.769764408584</v>
       </c>
       <c r="F32">
-        <v>174.90195</v>
+        <v>168.9066</v>
       </c>
       <c r="G32">
         <v>716.68799999999999</v>
       </c>
       <c r="H32">
-        <v>117.949001289639</v>
+        <v>120.18907852853501</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1644,16 +1636,16 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.22033846153846201</v>
+        <v>0.233566371681416</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>14.04</v>
+        <v>28.08</v>
       </c>
       <c r="H33">
-        <v>1.6459714322174701</v>
+        <v>1.86544856122699</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1670,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>4.4053054945054901</v>
+        <v>4.2234918879056096</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1679,7 +1671,7 @@
         <v>228.96</v>
       </c>
       <c r="H34">
-        <v>21.597672555128199</v>
+        <v>20.454601829533001</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1696,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1.1286923076923101</v>
+        <v>1.0302529498525099</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1705,7 +1697,7 @@
         <v>154.05000000000001</v>
       </c>
       <c r="H35">
-        <v>10.286355794053501</v>
+        <v>9.2262315312721093</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1716,22 +1708,22 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>6.5894999999999995E-2</v>
+        <v>5.7737499999999997E-2</v>
       </c>
       <c r="D36">
-        <v>0.80549999999999999</v>
+        <v>0.82055</v>
       </c>
       <c r="E36">
-        <v>4.1584544238754599</v>
+        <v>4.1868956834424802</v>
       </c>
       <c r="F36">
-        <v>4.1956249999999997</v>
+        <v>4.18511875</v>
       </c>
       <c r="G36">
         <v>92.078999999999994</v>
       </c>
       <c r="H36">
-        <v>8.8093891881787094</v>
+        <v>8.6022687490769894</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1745,19 +1737,19 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0.47493750000000001</v>
+        <v>0.45087500000000003</v>
       </c>
       <c r="E37">
-        <v>1.4240459706959701</v>
+        <v>1.3792804905117999</v>
       </c>
       <c r="F37">
-        <v>2.0049999999999999</v>
+        <v>1.7518750000000001</v>
       </c>
       <c r="G37">
         <v>16.763999999999999</v>
       </c>
       <c r="H37">
-        <v>2.2832616777667898</v>
+        <v>2.2974218485998801</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1768,22 +1760,22 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>5.37</v>
+        <v>5.0948437499999999</v>
       </c>
       <c r="D38">
-        <v>16.392192000000001</v>
+        <v>17.09</v>
       </c>
       <c r="E38">
-        <v>63.4995691161172</v>
+        <v>63.5018267317596</v>
       </c>
       <c r="F38">
-        <v>57.344999999999999</v>
+        <v>59.501249999999999</v>
       </c>
       <c r="G38">
-        <v>734.8</v>
+        <v>1155</v>
       </c>
       <c r="H38">
-        <v>114.83374345311699</v>
+        <v>117.30360101533</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1797,19 +1789,19 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="D39">
-        <v>0.36287999999999998</v>
+        <v>0.3468</v>
       </c>
       <c r="E39">
-        <v>0.99731103051648395</v>
+        <v>0.98243599633480805</v>
       </c>
       <c r="F39">
-        <v>1.2625999999999999</v>
+        <v>1.2670587499999999</v>
       </c>
       <c r="G39">
         <v>17.992000000000001</v>
       </c>
       <c r="H39">
-        <v>1.77932568738202</v>
+        <v>1.6887595509600899</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1820,22 +1812,22 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>3.7712500000000002</v>
+        <v>3.9212400000000001</v>
       </c>
       <c r="D40">
-        <v>12.6</v>
+        <v>12.57</v>
       </c>
       <c r="E40">
-        <v>22.4198535714286</v>
+        <v>22.3882550634277</v>
       </c>
       <c r="F40">
-        <v>29.232500000000002</v>
+        <v>27.732500000000002</v>
       </c>
       <c r="G40">
-        <v>177.12</v>
+        <v>275</v>
       </c>
       <c r="H40">
-        <v>26.883071391384298</v>
+        <v>28.290583709721201</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1846,22 +1838,22 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>7.4375</v>
+        <v>7.62</v>
       </c>
       <c r="D41">
-        <v>39.6</v>
+        <v>41.52</v>
       </c>
       <c r="E41">
-        <v>107.155679716484</v>
+        <v>108.09455708613601</v>
       </c>
       <c r="F41">
-        <v>143.91999999999999</v>
+        <v>152.14500000000001</v>
       </c>
       <c r="G41">
         <v>1128.33</v>
       </c>
       <c r="H41">
-        <v>163.28372848832899</v>
+        <v>159.30016103774901</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1872,22 +1864,22 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>38.950000000000003</v>
+        <v>39.15</v>
       </c>
       <c r="D42">
         <v>97.2</v>
       </c>
       <c r="E42">
-        <v>201.69018878717901</v>
+        <v>194.42754924671101</v>
       </c>
       <c r="F42">
-        <v>246.52860000000001</v>
+        <v>241.453125</v>
       </c>
       <c r="G42">
         <v>2590.8000000000002</v>
       </c>
       <c r="H42">
-        <v>285.31061556790303</v>
+        <v>271.601453690619</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1898,22 +1890,22 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>9.9375</v>
+        <v>10.08</v>
       </c>
       <c r="D43">
-        <v>90.7</v>
+        <v>100.75125</v>
       </c>
       <c r="E43">
-        <v>275.72454958937698</v>
+        <v>279.424186493614</v>
       </c>
       <c r="F43">
-        <v>358.77</v>
+        <v>387.93</v>
       </c>
       <c r="G43">
         <v>2852.28</v>
       </c>
       <c r="H43">
-        <v>425.28530345856899</v>
+        <v>419.431450134964</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1924,22 +1916,22 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>5.7599999999999998E-2</v>
+        <v>5.96E-2</v>
       </c>
       <c r="D44">
-        <v>0.315</v>
+        <v>0.33</v>
       </c>
       <c r="E44">
-        <v>0.74166921804029295</v>
+        <v>0.76667386903982304</v>
       </c>
       <c r="F44">
-        <v>0.83299999999999996</v>
+        <v>0.85568</v>
       </c>
       <c r="G44">
-        <v>12.82512</v>
+        <v>23.088239999999999</v>
       </c>
       <c r="H44">
-        <v>1.2795915664176001</v>
+        <v>1.6025822985346301</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1950,22 +1942,22 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>1.43E-2</v>
+        <v>1.303875E-2</v>
       </c>
       <c r="D45">
-        <v>4.7739999999999998E-2</v>
+        <v>4.2472500000000003E-2</v>
       </c>
       <c r="E45">
-        <v>9.3579465043589702E-2</v>
+        <v>9.06317503834808E-2</v>
       </c>
       <c r="F45">
-        <v>0.12422</v>
+        <v>0.12171</v>
       </c>
       <c r="G45">
         <v>1.23444</v>
       </c>
       <c r="H45">
-        <v>0.126605640089889</v>
+        <v>0.123691344148666</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1976,22 +1968,22 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>9.8500000000000004E-2</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="D46">
-        <v>1.3049999999999999</v>
+        <v>1.3743000000000001</v>
       </c>
       <c r="E46">
-        <v>8.8974856595238094</v>
+        <v>8.9841175389881993</v>
       </c>
       <c r="F46">
-        <v>9.2037499999999994</v>
+        <v>9.2306249999999999</v>
       </c>
       <c r="G46">
         <v>188.4708</v>
       </c>
       <c r="H46">
-        <v>18.2351403062661</v>
+        <v>17.843813245192401</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,19 +1997,19 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>0.32</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="E47">
-        <v>6.6499737783882802</v>
+        <v>6.2157678307772901</v>
       </c>
       <c r="F47">
-        <v>4.3559999999999999</v>
+        <v>3.6487500000000002</v>
       </c>
       <c r="G47">
-        <v>105.57</v>
+        <v>136.16</v>
       </c>
       <c r="H47">
-        <v>15.680858362473399</v>
+        <v>16.088900066441798</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2028,22 +2020,22 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>9.6249999999999999E-3</v>
+        <v>8.8050000000000003E-3</v>
       </c>
       <c r="D48">
-        <v>3.5279999999999999E-2</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="E48">
-        <v>0.11014319298278399</v>
+        <v>0.104574551268437</v>
       </c>
       <c r="F48">
-        <v>0.11072</v>
+        <v>0.11178</v>
       </c>
       <c r="G48">
         <v>3.7379099999999998</v>
       </c>
       <c r="H48">
-        <v>0.26356020042730999</v>
+        <v>0.232992703210333</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2054,13 +2046,13 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>1.2964597E-2</v>
+        <v>1.485E-2</v>
       </c>
       <c r="D49">
-        <v>5.0220000000000001E-2</v>
+        <v>5.2080000000000001E-2</v>
       </c>
       <c r="E49">
-        <v>0.136132927999634</v>
+        <v>0.13734805577433601</v>
       </c>
       <c r="F49">
         <v>0.17760000000000001</v>
@@ -2069,7 +2061,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="H49">
-        <v>0.19716614071056199</v>
+        <v>0.19439239931917099</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2080,13 +2072,13 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>7.7384999999999995E-2</v>
+        <v>7.6085E-2</v>
       </c>
       <c r="D50">
-        <v>0.36671999999999999</v>
+        <v>0.32690659999999999</v>
       </c>
       <c r="E50">
-        <v>1.55697542487839</v>
+        <v>1.5400297183510301</v>
       </c>
       <c r="F50">
         <v>1.55</v>
@@ -2095,7 +2087,7 @@
         <v>36.522174</v>
       </c>
       <c r="H50">
-        <v>3.44329202975592</v>
+        <v>3.3413898685042298</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2106,22 +2098,22 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>1.5423129000000001E-2</v>
+        <v>1.3616666750000001E-2</v>
       </c>
       <c r="D51">
-        <v>5.6000000000000001E-2</v>
+        <v>5.1771749999999998E-2</v>
       </c>
       <c r="E51">
-        <v>0.15249235351575099</v>
+        <v>0.14991445000590001</v>
       </c>
       <c r="F51">
-        <v>0.14976999999999999</v>
+        <v>0.15060499999999999</v>
       </c>
       <c r="G51">
-        <v>3.0939999999999999</v>
+        <v>3.8675000000000002</v>
       </c>
       <c r="H51">
-        <v>0.29298051191068503</v>
+        <v>0.31171300036786798</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2132,22 +2124,22 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>2.3562500000000002</v>
+        <v>2.2657500000000002</v>
       </c>
       <c r="D52">
-        <v>12</v>
+        <v>11.76</v>
       </c>
       <c r="E52">
-        <v>31.777519610989</v>
+        <v>30.772957388790601</v>
       </c>
       <c r="F52">
-        <v>37.15</v>
+        <v>35.662500000000001</v>
       </c>
       <c r="G52">
-        <v>617.95000000000005</v>
+        <v>772.4375</v>
       </c>
       <c r="H52">
-        <v>56.236906462592401</v>
+        <v>59.390179206183603</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2164,16 +2156,16 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>8.8931962637362592</v>
+        <v>9.4284409852507398</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
-        <v>601.79999999999995</v>
+        <v>752.25</v>
       </c>
       <c r="H53">
-        <v>39.898750263353499</v>
+        <v>45.465506248154298</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2184,22 +2176,22 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>2.2665000000000002</v>
+        <v>2.2078125000000002</v>
       </c>
       <c r="D54">
-        <v>9.6</v>
+        <v>8.9649999999999999</v>
       </c>
       <c r="E54">
-        <v>22.908587083516501</v>
+        <v>21.340978792920399</v>
       </c>
       <c r="F54">
-        <v>25.100543999999999</v>
+        <v>24.287500000000001</v>
       </c>
       <c r="G54">
-        <v>232.84800000000001</v>
+        <v>251.6</v>
       </c>
       <c r="H54">
-        <v>36.752958257294999</v>
+        <v>35.190180301199199</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2210,22 +2202,22 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>2.3562500000000002</v>
+        <v>2.2657500000000002</v>
       </c>
       <c r="D55">
-        <v>12.2</v>
+        <v>11.94</v>
       </c>
       <c r="E55">
-        <v>37.992300490109898</v>
+        <v>37.348114881415903</v>
       </c>
       <c r="F55">
-        <v>39</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="G55">
-        <v>1039.55</v>
+        <v>1299.4375</v>
       </c>
       <c r="H55">
-        <v>79.539381917008996</v>
+        <v>87.102165048485503</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,16 +2234,16 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>0.56809049560439595</v>
+        <v>0.56858189265191705</v>
       </c>
       <c r="F56">
         <v>0.28799999999999998</v>
       </c>
       <c r="G56">
-        <v>20.275919999999999</v>
+        <v>30.33</v>
       </c>
       <c r="H56">
-        <v>1.84206689273042</v>
+        <v>2.0546921512040601</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2265,10 +2257,10 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>3.36</v>
+        <v>3.2250000000000001</v>
       </c>
       <c r="E57">
-        <v>58.323172271062298</v>
+        <v>56.4121768456342</v>
       </c>
       <c r="F57">
         <v>57.628799999999998</v>
@@ -2277,7 +2269,7 @@
         <v>2224.9920000000002</v>
       </c>
       <c r="H57">
-        <v>159.86178475389099</v>
+        <v>162.34167102581799</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2294,16 +2286,16 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>32.685253964835198</v>
+        <v>30.327231509734499</v>
       </c>
       <c r="F58">
-        <v>4.87</v>
+        <v>7.9725000000000001</v>
       </c>
       <c r="G58">
         <v>2217.6</v>
       </c>
       <c r="H58">
-        <v>124.37430083839401</v>
+        <v>107.05757543627701</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2317,19 +2309,19 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>5.2</v>
+        <v>4.51</v>
       </c>
       <c r="E59">
-        <v>279.21773755970702</v>
+        <v>280.71489931401197</v>
       </c>
       <c r="F59">
-        <v>54.295999999999999</v>
+        <v>54.366500000000002</v>
       </c>
       <c r="G59">
-        <v>16380</v>
+        <v>16835</v>
       </c>
       <c r="H59">
-        <v>1163.2074431897699</v>
+        <v>1330.5818986895599</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2346,16 +2338,16 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>53.609014172161203</v>
+        <v>61.0708645993112</v>
       </c>
       <c r="F60">
-        <v>0.14149999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="G60">
-        <v>4172.3999999999996</v>
+        <v>6393.6</v>
       </c>
       <c r="H60">
-        <v>310.36705179790101</v>
+        <v>433.23007930500501</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2372,16 +2364,16 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>3.6692310989011001</v>
+        <v>3.4520581120944001</v>
       </c>
       <c r="F61">
-        <v>0.59699999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="G61">
         <v>182.52500000000001</v>
       </c>
       <c r="H61">
-        <v>13.402389023950899</v>
+        <v>13.145735928239199</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2398,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>227.56103159340699</v>
+        <v>240.447688974926</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2407,7 +2399,7 @@
         <v>31470.6</v>
       </c>
       <c r="H62">
-        <v>1742.3730439190799</v>
+        <v>1710.0978577706301</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2421,19 +2413,19 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>2.2679999999999998</v>
+        <v>1.35</v>
       </c>
       <c r="E63">
-        <v>216.07378783150199</v>
+        <v>199.32545750781699</v>
       </c>
       <c r="F63">
-        <v>71.683750000000003</v>
+        <v>63.5075</v>
       </c>
       <c r="G63">
         <v>7866.72</v>
       </c>
       <c r="H63">
-        <v>839.59937808400605</v>
+        <v>762.92657956849598</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2444,22 +2436,22 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>2.9684550000000001E-2</v>
+        <v>2.41E-2</v>
       </c>
       <c r="D64">
-        <v>0.18</v>
+        <v>0.16985</v>
       </c>
       <c r="E64">
-        <v>0.68098255187545798</v>
+        <v>0.69974434243510297</v>
       </c>
       <c r="F64">
-        <v>0.78200000000000003</v>
+        <v>0.66921750000000002</v>
       </c>
       <c r="G64">
-        <v>8.3469999999999995</v>
+        <v>11.396000000000001</v>
       </c>
       <c r="H64">
-        <v>1.1744037581673801</v>
+        <v>1.3881905850417899</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2470,22 +2462,22 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>0.127</v>
+        <v>5.6774999999999999E-2</v>
       </c>
       <c r="D65">
-        <v>1.5442499999999999</v>
+        <v>1.4437500000000001</v>
       </c>
       <c r="E65">
-        <v>15.0001575263736</v>
+        <v>14.6451261389086</v>
       </c>
       <c r="F65">
-        <v>8.5950000000000006</v>
+        <v>8.2829999999999995</v>
       </c>
       <c r="G65">
-        <v>328.77600000000001</v>
+        <v>416.62</v>
       </c>
       <c r="H65">
-        <v>40.623547345208998</v>
+        <v>43.113598020962698</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2502,16 +2494,16 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>24.105143389011001</v>
+        <v>24.433734586430699</v>
       </c>
       <c r="F66">
-        <v>9.42</v>
+        <v>9.6</v>
       </c>
       <c r="G66">
         <v>840</v>
       </c>
       <c r="H66">
-        <v>82.564907693760702</v>
+        <v>80.392597419860806</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2522,22 +2514,22 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>1.04625E-2</v>
+        <v>9.0806250000000002E-3</v>
       </c>
       <c r="D67">
         <v>0.31979999999999997</v>
       </c>
       <c r="E67">
-        <v>1.6649470378164799</v>
+        <v>1.68298389023451</v>
       </c>
       <c r="F67">
-        <v>1.794055</v>
+        <v>1.8517275</v>
       </c>
       <c r="G67">
         <v>20.178629999999998</v>
       </c>
       <c r="H67">
-        <v>3.0970200476288801</v>
+        <v>3.0826955493084802</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2554,16 +2546,16 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>2.97207985142857E-2</v>
+        <v>3.0028061281710899E-2</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G68">
         <v>0.58904999999999996</v>
       </c>
       <c r="H68">
-        <v>8.6508268263486995E-2</v>
+        <v>8.6461632101525396E-2</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2580,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>1.97613442241758E-2</v>
+        <v>2.0596017395280199E-2</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2589,7 +2581,7 @@
         <v>0.45045000000000002</v>
       </c>
       <c r="H69">
-        <v>5.8593832545633301E-2</v>
+        <v>6.0600818384297699E-2</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,16 +2598,16 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>1.6086567092307699E-2</v>
+        <v>1.59379376902655E-2</v>
       </c>
       <c r="F70">
-        <v>2.5415625E-3</v>
+        <v>2.52203125E-3</v>
       </c>
       <c r="G70">
         <v>0.40260000000000001</v>
       </c>
       <c r="H70">
-        <v>4.4317459190649201E-2</v>
+        <v>4.4386952911693103E-2</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2632,16 +2624,16 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>3.08393907648352E-2</v>
+        <v>3.2450847091445398E-2</v>
       </c>
       <c r="F71">
-        <v>7.7287500000000004E-3</v>
+        <v>6.7012499999999997E-3</v>
       </c>
       <c r="G71">
-        <v>0.63629999999999998</v>
+        <v>1.120959</v>
       </c>
       <c r="H71">
-        <v>8.6460974957578901E-2</v>
+        <v>9.6461850442441696E-2</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,16 +2650,16 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>4.1057939652747302E-2</v>
+        <v>4.0056139087020701E-2</v>
       </c>
       <c r="F72">
-        <v>8.1606249999999995E-3</v>
+        <v>7.9749999999999995E-3</v>
       </c>
       <c r="G72">
         <v>2.5424799999999999</v>
       </c>
       <c r="H72">
-        <v>0.15351669427568301</v>
+        <v>0.140228218782291</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2681,19 +2673,19 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>3.2599999999999999E-3</v>
+        <v>3.2274999999999999E-3</v>
       </c>
       <c r="E73">
-        <v>0.13460847921465199</v>
+        <v>0.13708072674041299</v>
       </c>
       <c r="F73">
-        <v>3.8030000000000001E-2</v>
+        <v>3.7589999999999998E-2</v>
       </c>
       <c r="G73">
         <v>2.2101000000000002</v>
       </c>
       <c r="H73">
-        <v>0.34436318309285902</v>
+        <v>0.34793977553483502</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2704,22 +2696,22 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>9.1537500000000004E-3</v>
+        <v>7.4354167499999999E-3</v>
       </c>
       <c r="D74">
-        <v>0.21804000000000001</v>
+        <v>0.22036</v>
       </c>
       <c r="E74">
-        <v>0.94197356926520104</v>
+        <v>0.95091500632890902</v>
       </c>
       <c r="F74">
-        <v>1.058746</v>
+        <v>1.1174949999999999</v>
       </c>
       <c r="G74">
-        <v>10.60848</v>
+        <v>10.75032</v>
       </c>
       <c r="H74">
-        <v>1.6724798998419801</v>
+        <v>1.6665256263205701</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2730,22 +2722,22 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>7.5000000000000002E-4</v>
+        <v>7.4425000000000001E-4</v>
       </c>
       <c r="D75">
-        <v>4.77425E-2</v>
+        <v>4.8171249999999999E-2</v>
       </c>
       <c r="E75">
-        <v>0.38936970824652001</v>
+        <v>0.39352922673451302</v>
       </c>
       <c r="F75">
-        <v>0.35372999999999999</v>
+        <v>0.39138000000000001</v>
       </c>
       <c r="G75">
-        <v>4.9139999999999997</v>
+        <v>6.2868959999999996</v>
       </c>
       <c r="H75">
-        <v>0.79283937972677898</v>
+        <v>0.78961863191164705</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2756,22 +2748,22 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>6.8981249999999997E-3</v>
+        <v>7.6800000000000002E-3</v>
       </c>
       <c r="D76">
-        <v>0.34620000000000001</v>
+        <v>0.37278600000000001</v>
       </c>
       <c r="E76">
-        <v>2.1338093680476198</v>
+        <v>2.1239170764188802</v>
       </c>
       <c r="F76">
-        <v>2.5689899999999999</v>
+        <v>2.5513949999999999</v>
       </c>
       <c r="G76">
-        <v>22.714379999999998</v>
+        <v>25.2044</v>
       </c>
       <c r="H76">
-        <v>3.6371124630337102</v>
+        <v>3.7572282868300602</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2785,19 +2777,19 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>4.7999999999999996E-3</v>
+        <v>4.8664320000000004E-3</v>
       </c>
       <c r="E77">
-        <v>8.0843190130402906E-2</v>
+        <v>7.8554390353982304E-2</v>
       </c>
       <c r="F77">
-        <v>4.5644999999999998E-2</v>
+        <v>4.8282499999999999E-2</v>
       </c>
       <c r="G77">
-        <v>1.4029799999999999</v>
+        <v>1.585332</v>
       </c>
       <c r="H77">
-        <v>0.19233983742737501</v>
+        <v>0.18830275430297899</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2808,22 +2800,22 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>4.5500000000000002E-3</v>
+        <v>5.4226562500000004E-3</v>
       </c>
       <c r="D78">
-        <v>0.32665</v>
+        <v>0.32772499999999999</v>
       </c>
       <c r="E78">
-        <v>1.9772198888703301</v>
+        <v>1.9751138564483799</v>
       </c>
       <c r="F78">
-        <v>2.4308700000000001</v>
+        <v>2.4221400000000002</v>
       </c>
       <c r="G78">
-        <v>22.086739999999999</v>
+        <v>24.6938</v>
       </c>
       <c r="H78">
-        <v>3.40007532178933</v>
+        <v>3.5361162363968099</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2840,16 +2832,16 @@
         <v>3.5199999999999999E-4</v>
       </c>
       <c r="E79">
-        <v>3.9226217786813199E-2</v>
+        <v>3.5388466883480803E-2</v>
       </c>
       <c r="F79">
-        <v>2.3640000000000001E-2</v>
+        <v>2.1524999999999999E-2</v>
       </c>
       <c r="G79">
         <v>1.877904</v>
       </c>
       <c r="H79">
-        <v>0.15067279031589101</v>
+        <v>0.140623195447032</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2866,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>6.8170178021978002E-3</v>
+        <v>7.4278010324483803E-3</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -2875,7 +2867,7 @@
         <v>1.570592</v>
       </c>
       <c r="H80">
-        <v>7.5691032135881006E-2</v>
+        <v>8.5462860488581399E-2</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2886,22 +2878,22 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>2.4629999999999999E-2</v>
+        <v>2.40328125E-2</v>
       </c>
       <c r="D81">
-        <v>0.27481499999999998</v>
+        <v>0.25278499999999998</v>
       </c>
       <c r="E81">
-        <v>1.70404679886044</v>
+        <v>1.68245484812242</v>
       </c>
       <c r="F81">
-        <v>1.805308125</v>
+        <v>1.7485649999999999</v>
       </c>
       <c r="G81">
         <v>34.757800000000003</v>
       </c>
       <c r="H81">
-        <v>3.3643881393166701</v>
+        <v>3.4368316454191201</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -2912,22 +2904,22 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>1.6181250000000001E-2</v>
+        <v>1.7437500000000002E-2</v>
       </c>
       <c r="D82">
-        <v>0.19592000000000001</v>
+        <v>0.17155999999999999</v>
       </c>
       <c r="E82">
-        <v>1.4520722359164799</v>
+        <v>1.4371683841371701</v>
       </c>
       <c r="F82">
-        <v>1.486194</v>
+        <v>1.436971875</v>
       </c>
       <c r="G82">
         <v>30.43656</v>
       </c>
       <c r="H82">
-        <v>2.92701603649602</v>
+        <v>2.9861549001854</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -2941,19 +2933,19 @@
         <v>2.6099999999999999E-3</v>
       </c>
       <c r="D83">
-        <v>2.964E-2</v>
+        <v>2.7026250000000002E-2</v>
       </c>
       <c r="E83">
-        <v>0.18533333557326001</v>
+        <v>0.18274779323451301</v>
       </c>
       <c r="F83">
-        <v>0.16647000000000001</v>
+        <v>0.15553500000000001</v>
       </c>
       <c r="G83">
         <v>4.54</v>
       </c>
       <c r="H83">
-        <v>0.42525767675773002</v>
+        <v>0.44666765822627102</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2970,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>3.1693516483516501E-3</v>
+        <v>2.9801102507374601E-3</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2979,7 +2971,7 @@
         <v>0.324324</v>
       </c>
       <c r="H84">
-        <v>2.5862531751432601E-2</v>
+        <v>2.5561225256520499E-2</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,16 +2988,16 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>1.22055631956044E-2</v>
+        <v>1.2319835943952801E-2</v>
       </c>
       <c r="F85">
-        <v>2.3525759999999999E-3</v>
+        <v>2.3762879999999998E-3</v>
       </c>
       <c r="G85">
         <v>0.42</v>
       </c>
       <c r="H85">
-        <v>4.35659669267476E-2</v>
+        <v>4.2666227390403801E-2</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="E86">
-        <v>1.22543171692308E-2</v>
+        <v>1.1512454737463099E-2</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -3031,7 +3023,7 @@
         <v>1.097712</v>
       </c>
       <c r="H86">
-        <v>8.1481860457498403E-2</v>
+        <v>8.1126478721237405E-2</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3048,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>3.8513203296703302E-3</v>
+        <v>3.7064929941002999E-3</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -3057,7 +3049,7 @@
         <v>0.26082</v>
       </c>
       <c r="H87">
-        <v>2.2501129601019101E-2</v>
+        <v>2.1582173897575E-2</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3074,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <v>2.3558692967033001E-2</v>
+        <v>2.17856840707965E-2</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3083,7 +3075,7 @@
         <v>1.7781119999999999</v>
       </c>
       <c r="H88">
-        <v>0.14802882249593799</v>
+        <v>0.143209208465719</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3100,16 +3092,16 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>0.83117673582417595</v>
+        <v>0.73308167551622405</v>
       </c>
       <c r="F89">
-        <v>3.2000000000000001E-2</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="G89">
         <v>45.246600000000001</v>
       </c>
       <c r="H89">
-        <v>4.0026096668761104</v>
+        <v>3.57967155770138</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3123,19 +3115,19 @@
         <v>1.647</v>
       </c>
       <c r="D90">
-        <v>7.16</v>
+        <v>7.3475625000000004</v>
       </c>
       <c r="E90">
-        <v>29.7293098216484</v>
+        <v>29.633659539587001</v>
       </c>
       <c r="F90">
-        <v>27.236999999999998</v>
+        <v>27.75</v>
       </c>
       <c r="G90">
         <v>574.5</v>
       </c>
       <c r="H90">
-        <v>63.555478785564198</v>
+        <v>62.115808060020903</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3152,16 +3144,16 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>6.2001362637362598E-2</v>
+        <v>7.0869188790560506E-2</v>
       </c>
       <c r="F91">
         <v>0</v>
       </c>
       <c r="G91">
-        <v>8.3469999999999995</v>
+        <v>10.43375</v>
       </c>
       <c r="H91">
-        <v>0.65770607512027901</v>
+        <v>0.758307389012984</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3178,16 +3170,16 @@
         <v>0</v>
       </c>
       <c r="E92">
-        <v>0.10256341758241801</v>
+        <v>9.3531268436578205E-2</v>
       </c>
       <c r="F92">
         <v>0</v>
       </c>
       <c r="G92">
-        <v>9.2565000000000008</v>
+        <v>11.570625</v>
       </c>
       <c r="H92">
-        <v>0.612249524540463</v>
+        <v>0.67891535192333996</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3204,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="E93">
-        <v>4.21871659340659E-2</v>
+        <v>3.9562590707964598E-2</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -3213,7 +3205,7 @@
         <v>1.5811999999999999</v>
       </c>
       <c r="H93">
-        <v>0.20342692266961601</v>
+        <v>0.18575954250306001</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3230,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <v>1.2973681318681299E-2</v>
+        <v>1.15554203539823E-2</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -3239,7 +3231,7 @@
         <v>1.5555000000000001</v>
       </c>
       <c r="H94">
-        <v>0.10401851294963201</v>
+        <v>9.23028140235682E-2</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3256,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>2.4170346153846198E-2</v>
+        <v>2.3012379793510299E-2</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -3265,7 +3257,7 @@
         <v>1.5811999999999999</v>
       </c>
       <c r="H95">
-        <v>0.15051158565345699</v>
+        <v>0.13882203771313201</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3282,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="E96">
-        <v>5.0431384615384602E-3</v>
+        <v>4.9947905604719803E-3</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -3291,7 +3283,7 @@
         <v>1.0416000000000001</v>
       </c>
       <c r="H96">
-        <v>5.8183723687674098E-2</v>
+        <v>6.0984534227335498E-2</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3308,16 +3300,16 @@
         <v>0</v>
       </c>
       <c r="E97">
-        <v>0.183637434058608</v>
+        <v>0.17453959623451301</v>
       </c>
       <c r="F97">
-        <v>0.18699687500000001</v>
+        <v>0.15056249999999999</v>
       </c>
       <c r="G97">
         <v>4.0289999999999999</v>
       </c>
       <c r="H97">
-        <v>0.40640427345630298</v>
+        <v>0.42315702385696002</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3334,16 +3326,16 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>2.8373278388278401E-2</v>
+        <v>2.94847130044248E-2</v>
       </c>
       <c r="F98">
         <v>0</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="H98">
-        <v>0.121045654795013</v>
+        <v>0.129883762559902</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3360,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="E99">
-        <v>2.9702274725274699E-2</v>
+        <v>2.9257197640117999E-2</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3369,7 +3361,7 @@
         <v>1.2726</v>
       </c>
       <c r="H99">
-        <v>0.13242520596689999</v>
+        <v>0.132242001446743</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3386,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="E100">
-        <v>1.6696175824175801E-2</v>
+        <v>1.5581025073746301E-2</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -3395,7 +3387,7 @@
         <v>1.2726</v>
       </c>
       <c r="H100">
-        <v>0.109066336318511</v>
+        <v>9.6569939400844004E-2</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3412,16 +3404,16 @@
         <v>0</v>
       </c>
       <c r="E101">
-        <v>1.3006098901098899E-2</v>
+        <v>1.36761725663717E-2</v>
       </c>
       <c r="F101">
         <v>0</v>
       </c>
       <c r="G101">
-        <v>0.96</v>
+        <v>1.1839999999999999</v>
       </c>
       <c r="H101">
-        <v>7.5759216264491697E-2</v>
+        <v>8.9992385738489999E-2</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3438,7 +3430,7 @@
         <v>0</v>
       </c>
       <c r="E102">
-        <v>3.4935576923076903E-2</v>
+        <v>3.3553742625368699E-2</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -3447,7 +3439,7 @@
         <v>4.0289999999999999</v>
       </c>
       <c r="H102">
-        <v>0.274663029463382</v>
+        <v>0.24519616863433399</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3464,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="E103">
-        <v>3.1385934065934103E-2</v>
+        <v>2.9797566371681398E-2</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -3473,7 +3465,7 @@
         <v>4.0289999999999999</v>
       </c>
       <c r="H103">
-        <v>0.27273739225143001</v>
+        <v>0.24259650953370901</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3490,16 +3482,16 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>3.5496428571428601E-3</v>
+        <v>3.7561762536873198E-3</v>
       </c>
       <c r="F104">
         <v>0</v>
       </c>
       <c r="G104">
-        <v>0.42480000000000001</v>
+        <v>0.504</v>
       </c>
       <c r="H104">
-        <v>2.9917274263588998E-2</v>
+        <v>3.32390783387859E-2</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3516,16 +3508,16 @@
         <v>0</v>
       </c>
       <c r="E105">
-        <v>9.0626304021977994E-2</v>
+        <v>8.2243942964601802E-2</v>
       </c>
       <c r="F105">
-        <v>4.2999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="G105">
         <v>1.7301</v>
       </c>
       <c r="H105">
-        <v>0.23140509946787699</v>
+        <v>0.23150585993107001</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -3542,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="E106">
-        <v>2.0269505494505499E-2</v>
+        <v>1.7814417404129802E-2</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -3551,7 +3543,7 @@
         <v>0.76200000000000001</v>
       </c>
       <c r="H106">
-        <v>9.3886849311277595E-2</v>
+        <v>8.6304411473148601E-2</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3568,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="E107">
-        <v>0.32630312967032998</v>
+        <v>0.32681469929203499</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -3577,7 +3569,7 @@
         <v>7.7561999999999998</v>
       </c>
       <c r="H107">
-        <v>0.893865034072162</v>
+        <v>0.87422071265078904</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3594,16 +3586,16 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <v>5.1423296703296699E-2</v>
+        <v>5.763901179941E-2</v>
       </c>
       <c r="F108">
         <v>0</v>
       </c>
       <c r="G108">
-        <v>2.6562000000000001</v>
+        <v>2.8593000000000002</v>
       </c>
       <c r="H108">
-        <v>0.295675707703003</v>
+        <v>0.32512860094142698</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3620,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="E109">
-        <v>0.274879832967033</v>
+        <v>0.26917568749262499</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3629,7 +3621,7 @@
         <v>7.7561999999999998</v>
       </c>
       <c r="H109">
-        <v>0.84908354257936602</v>
+        <v>0.82056236655831505</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3646,16 +3638,16 @@
         <v>0</v>
       </c>
       <c r="E110">
-        <v>0.46907671153846198</v>
+        <v>0.48788171644542799</v>
       </c>
       <c r="F110">
-        <v>4.36E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="G110">
         <v>11.328659999999999</v>
       </c>
       <c r="H110">
-        <v>1.3170826662869299</v>
+        <v>1.36042445137458</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3672,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="E111">
-        <v>0.30511887912087898</v>
+        <v>0.32355134955752202</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3681,7 +3673,7 @@
         <v>11.328659999999999</v>
       </c>
       <c r="H111">
-        <v>1.2191833102405101</v>
+        <v>1.26584559046238</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3698,16 +3690,16 @@
         <v>0</v>
       </c>
       <c r="E112">
-        <v>5.9495780219780199E-2</v>
+        <v>8.02269321533923E-2</v>
       </c>
       <c r="F112">
         <v>0</v>
       </c>
       <c r="G112">
-        <v>3.9123000000000001</v>
+        <v>11.15856</v>
       </c>
       <c r="H112">
-        <v>0.413334839713423</v>
+        <v>0.66485943670930603</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3724,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>4.12323296703297E-2</v>
+        <v>3.5907979351032397E-2</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -3733,7 +3725,7 @@
         <v>6.0045299999999999</v>
       </c>
       <c r="H113">
-        <v>0.36690414697832302</v>
+        <v>0.31787367050758902</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3776,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="E115">
-        <v>2.89520879120879E-2</v>
+        <v>3.86432079646018E-2</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -3785,7 +3777,7 @@
         <v>4.0362</v>
       </c>
       <c r="H115">
-        <v>0.29987157521192398</v>
+        <v>0.34331292550805198</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3802,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="E116">
-        <v>0.114842175824176</v>
+        <v>9.4681725663716798E-2</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -3811,7 +3803,7 @@
         <v>11.328659999999999</v>
       </c>
       <c r="H116">
-        <v>0.88649490690928001</v>
+        <v>0.79411545738552003</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3828,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>6.0596505494505501E-2</v>
+        <v>7.4091504424778798E-2</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -3837,7 +3829,7 @@
         <v>9.4688999999999997</v>
       </c>
       <c r="H117">
-        <v>0.56883569118580801</v>
+        <v>0.59366284470327901</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3854,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <v>7.1989428571428593E-2</v>
+        <v>6.9138171091445405E-2</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -3863,7 +3855,7 @@
         <v>4.5</v>
       </c>
       <c r="H118">
-        <v>0.40564739094312902</v>
+        <v>0.38497911403903601</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3880,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="E119">
-        <v>4.1272197802197798E-2</v>
+        <v>3.6425479351032401E-2</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -3889,7 +3881,7 @@
         <v>3.3557999999999999</v>
       </c>
       <c r="H119">
-        <v>0.27069501463621998</v>
+        <v>0.24817020756856001</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -3906,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="E120">
-        <v>5.0696206043955999E-2</v>
+        <v>5.8766716445427698E-2</v>
       </c>
       <c r="F120">
         <v>0</v>
@@ -3915,7 +3907,7 @@
         <v>3.5249999999999999</v>
       </c>
       <c r="H120">
-        <v>0.29353211951742703</v>
+        <v>0.33870596534386499</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3932,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="E121">
-        <v>8.1450659340659301E-2</v>
+        <v>7.1534070796460195E-2</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -3941,7 +3933,7 @@
         <v>3.0099</v>
       </c>
       <c r="H121">
-        <v>0.37573351021922002</v>
+        <v>0.34566037600754301</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -3958,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="E122">
-        <v>0.11132633516483501</v>
+        <v>0.11160026917404101</v>
       </c>
       <c r="F122">
         <v>0</v>
@@ -3967,7 +3959,7 @@
         <v>2.42</v>
       </c>
       <c r="H122">
-        <v>0.33753968312618998</v>
+        <v>0.33406055602028401</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3984,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="E123">
-        <v>4.4961780219780201E-2</v>
+        <v>4.1743001474926301E-2</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -3993,7 +3985,7 @@
         <v>2.0007999999999999</v>
       </c>
       <c r="H123">
-        <v>0.196346543977341</v>
+        <v>0.18387773407164301</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4010,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="E124">
-        <v>7.9629945054944997E-3</v>
+        <v>6.2675553097345099E-3</v>
       </c>
       <c r="F124">
         <v>0</v>
@@ -4019,7 +4011,7 @@
         <v>1.50675</v>
       </c>
       <c r="H124">
-        <v>8.3913618571575394E-2</v>
+        <v>7.1843990568479704E-2</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4036,7 +4028,7 @@
         <v>0</v>
       </c>
       <c r="E125">
-        <v>4.64798901098901E-2</v>
+        <v>5.00782669616519E-2</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -4045,7 +4037,7 @@
         <v>2.42</v>
       </c>
       <c r="H125">
-        <v>0.24559154276336101</v>
+        <v>0.25514400767162898</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4062,16 +4054,16 @@
         <v>0</v>
       </c>
       <c r="E126">
-        <v>2.6436897859780202</v>
+        <v>2.5704986412094399</v>
       </c>
       <c r="F126">
-        <v>2.1639750000000002</v>
+        <v>1.8959999999999999</v>
       </c>
       <c r="G126">
-        <v>56.363999999999997</v>
+        <v>59.496000000000002</v>
       </c>
       <c r="H126">
-        <v>5.9818643489208201</v>
+        <v>6.3170669863264202</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4088,16 +4080,16 @@
         <v>0</v>
       </c>
       <c r="E127">
-        <v>1.88593003927473</v>
+        <v>1.9229228921681401</v>
       </c>
       <c r="F127">
-        <v>0.35249999999999998</v>
+        <v>0.53381250000000002</v>
       </c>
       <c r="G127">
         <v>38.674999999999997</v>
       </c>
       <c r="H127">
-        <v>4.88325843113447</v>
+        <v>4.7305969854712702</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4114,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="E128">
-        <v>0.461092414835165</v>
+        <v>0.47523962529498498</v>
       </c>
       <c r="F128">
         <v>0</v>
@@ -4123,7 +4115,7 @@
         <v>21.352499999999999</v>
       </c>
       <c r="H128">
-        <v>1.75393319779048</v>
+        <v>1.70488637339573</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4140,16 +4132,16 @@
         <v>0</v>
       </c>
       <c r="E129">
-        <v>1.5812307692307698E-2</v>
+        <v>1.6756637168141599E-2</v>
       </c>
       <c r="F129">
         <v>0</v>
       </c>
       <c r="G129">
-        <v>1.008</v>
+        <v>2.016</v>
       </c>
       <c r="H129">
-        <v>0.118142124622429</v>
+        <v>0.133867300225335</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4235,25 +4227,25 @@
         <v>140</v>
       </c>
       <c r="B133">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C133">
         <v>31</v>
       </c>
       <c r="D133">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E133">
-        <v>42.916483516483503</v>
+        <v>43.554572271386398</v>
       </c>
       <c r="F133">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G133">
         <v>71</v>
       </c>
       <c r="H133">
-        <v>14.769508593141399</v>
+        <v>15.1110845297786</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4261,25 +4253,25 @@
         <v>141</v>
       </c>
       <c r="B134">
-        <v>48</v>
+        <v>53.9</v>
       </c>
       <c r="C134">
-        <v>53.9</v>
+        <v>60</v>
       </c>
       <c r="D134">
         <v>73</v>
       </c>
       <c r="E134">
-        <v>69.751648351648399</v>
+        <v>72.247197640118003</v>
       </c>
       <c r="F134">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G134">
-        <v>99</v>
+        <v>90.7</v>
       </c>
       <c r="H134">
-        <v>16.2066090466936</v>
+        <v>11.402345613434401</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4296,16 +4288,16 @@
         <v>169</v>
       </c>
       <c r="E135">
-        <v>168.75142857142899</v>
+        <v>168.720943952802</v>
       </c>
       <c r="F135">
-        <v>177.8</v>
+        <v>175</v>
       </c>
       <c r="G135">
         <v>186</v>
       </c>
       <c r="H135">
-        <v>10.440027656577699</v>
+        <v>9.9149382691050008</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4313,25 +4305,25 @@
         <v>143</v>
       </c>
       <c r="B136">
-        <v>19</v>
+        <v>18.7898335</v>
       </c>
       <c r="C136">
-        <v>21</v>
+        <v>22.835009830000001</v>
       </c>
       <c r="D136">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E136">
-        <v>24.393406593406599</v>
+        <v>25.4125019802065</v>
       </c>
       <c r="F136">
-        <v>27</v>
+        <v>27.814077189999999</v>
       </c>
       <c r="G136">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H136">
-        <v>4.2204088314239998</v>
+        <v>3.80900260566691</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4339,25 +4331,25 @@
         <v>144</v>
       </c>
       <c r="B137">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C137">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D137">
         <v>85</v>
       </c>
       <c r="E137">
-        <v>85.374725274725293</v>
+        <v>84.632005899705007</v>
       </c>
       <c r="F137">
         <v>90</v>
       </c>
       <c r="G137">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="H137">
-        <v>7.3831364198098601</v>
+        <v>10.304445088644901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>